<commit_message>
Ruan: backup in 20171025
</commit_message>
<xml_diff>
--- a/BOM/IGuide_component.xlsx
+++ b/BOM/IGuide_component.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186">
   <si>
     <t>类型</t>
   </si>
@@ -472,18 +472,143 @@
 -
  1A  </t>
   </si>
+  <si>
+    <t>NO.</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Manufacturer No.</t>
+  </si>
+  <si>
+    <t>No./set</t>
+  </si>
+  <si>
+    <t>DIGI-KEY prices</t>
+  </si>
+  <si>
+    <t>RMB</t>
+  </si>
+  <si>
+    <t>8PIN</t>
+  </si>
+  <si>
+    <t>ATtiny45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTINY45V-10SUR  2,000 - 立即发货 
+  ¥ 10.49985 </t>
+  </si>
+  <si>
+    <t>定制线圈</t>
+  </si>
+  <si>
+    <t>未知</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V X7R 0805</t>
+  </si>
+  <si>
+    <t>C0805C106J8RACAUTO</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,500  0 
+ 原厂标准交货期 31 周   ¥ 1.71596 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1µF  ±5%  25V  X7R  </t>
+  </si>
+  <si>
+    <t>C0805C105J3RACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,500  95,000 - 立即发货 
+  ¥ 2.17797 </t>
+  </si>
+  <si>
+    <t>C1206C124J5RACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,000 ¥ 0.93718 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTC THERMISTOR 4.7K OHM 1% 0805 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,000     ¥ 3.22398 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 10K OHM 1% 1/16W 0402 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-0710KL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,000  13,010,000 - 立即发货 
+  ¥ 0.01260 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 0 OHM JUMPER 1/16W 0402 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402JR-070RL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,000  15,950,000 - 立即发货 
+  ¥ 0.00779  </t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 200MA SC70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAT54SWF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nexperia USA Inc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET N/P-CH 30V TSMT8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohm Semiconductor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,000  0   ¥ 2.21636 </t>
+  </si>
+  <si>
+    <t>BC817-40W</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,000  6,000 - 立即发货 
+  ¥ 0.40479 </t>
+  </si>
+  <si>
+    <t>BC807-40W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,000  33,000 - 立即发货 
+  ¥ 0.40479 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,10 +617,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -513,11 +713,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -530,10 +736,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -545,17 +751,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -569,72 +767,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -663,192 +801,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -948,6 +1086,120 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -964,26 +1216,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,17 +1261,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1027,26 +1288,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1058,10 +1310,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1070,137 +1322,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1260,6 +1512,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1328,7 +1622,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>526415</xdr:colOff>
+      <xdr:colOff>480695</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>313055</xdr:rowOff>
     </xdr:to>
@@ -1647,19 +1941,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G95" sqref="A82:G95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="24.25" customWidth="1"/>
     <col min="2" max="2" width="27.2222222222222" style="1" customWidth="1"/>
     <col min="3" max="4" width="37.6666666666667" customWidth="1"/>
     <col min="5" max="5" width="33.2222222222222" customWidth="1"/>
     <col min="6" max="6" width="66.3333333333333" customWidth="1"/>
+    <col min="7" max="7" width="9.66666666666667"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
@@ -2417,6 +2712,300 @@
     <row r="66" ht="43.2" spans="3:3">
       <c r="C66" s="19" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="F82" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="G82" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" ht="28.8" spans="1:7">
+      <c r="A83" s="24">
+        <v>59</v>
+      </c>
+      <c r="B83" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C83" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D83" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E83" s="26">
+        <v>1</v>
+      </c>
+      <c r="F83" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="G83" s="23">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="84" ht="15.6" spans="1:7">
+      <c r="A84" s="24">
+        <v>75</v>
+      </c>
+      <c r="B84" s="25"/>
+      <c r="C84" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D84" s="25"/>
+      <c r="E84" s="26">
+        <v>1</v>
+      </c>
+      <c r="F84" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="G84" s="23"/>
+    </row>
+    <row r="85" ht="31.2" spans="1:7">
+      <c r="A85" s="24">
+        <v>10</v>
+      </c>
+      <c r="B85" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C85" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="D85" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="E85" s="26">
+        <v>2</v>
+      </c>
+      <c r="F85" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="G85" s="23">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="86" ht="28.8" spans="1:7">
+      <c r="A86" s="24">
+        <v>6</v>
+      </c>
+      <c r="B86" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C86" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D86" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="E86" s="26">
+        <v>1</v>
+      </c>
+      <c r="F86" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G86" s="23">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="87" ht="15.6" spans="1:7">
+      <c r="A87" s="24">
+        <v>19</v>
+      </c>
+      <c r="B87" s="29"/>
+      <c r="C87" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D87" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E87" s="26">
+        <v>2</v>
+      </c>
+      <c r="F87" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G87" s="23">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="88" ht="31.2" spans="1:7">
+      <c r="A88" s="24">
+        <v>50</v>
+      </c>
+      <c r="B88" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D88" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E88" s="26">
+        <v>1</v>
+      </c>
+      <c r="F88" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G88" s="23">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="89" ht="31.2" spans="1:7">
+      <c r="A89" s="24">
+        <v>44</v>
+      </c>
+      <c r="B89" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C89" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D89" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E89" s="26">
+        <v>1</v>
+      </c>
+      <c r="F89" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="G89" s="23">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="90" ht="31.2" spans="1:7">
+      <c r="A90" s="24">
+        <v>41</v>
+      </c>
+      <c r="B90" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C90" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D90" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E90" s="26">
+        <v>7</v>
+      </c>
+      <c r="F90" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="G90" s="23">
+        <v>0.05453</v>
+      </c>
+    </row>
+    <row r="91" ht="31.2" spans="1:7">
+      <c r="A91" s="24">
+        <v>32</v>
+      </c>
+      <c r="B91" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C91" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="E91" s="26">
+        <v>1</v>
+      </c>
+      <c r="F91" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="G91" s="23">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="92" ht="15.6" spans="1:7">
+      <c r="A92" s="24">
+        <v>33</v>
+      </c>
+      <c r="B92" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D92" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="E92" s="26">
+        <v>1</v>
+      </c>
+      <c r="F92" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G92" s="23">
+        <v>2.216</v>
+      </c>
+    </row>
+    <row r="93" ht="28.8" spans="1:7">
+      <c r="A93" s="24">
+        <v>81</v>
+      </c>
+      <c r="B93" s="25"/>
+      <c r="C93" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D93" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="E93" s="26">
+        <v>1</v>
+      </c>
+      <c r="F93" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="G93" s="23">
+        <v>0.405</v>
+      </c>
+    </row>
+    <row r="94" ht="29.55" spans="1:7">
+      <c r="A94" s="31">
+        <v>82</v>
+      </c>
+      <c r="B94" s="32"/>
+      <c r="C94" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="D94" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="E94" s="33">
+        <v>1</v>
+      </c>
+      <c r="F94" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="G94" s="23">
+        <v>0.405</v>
+      </c>
+    </row>
+    <row r="95" spans="6:7">
+      <c r="F95" s="23"/>
+      <c r="G95" s="23">
+        <f>SUM(G83:G94)</f>
+        <v>24.52253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>